<commit_message>
100% diagnosis, changes in a few functions
</commit_message>
<xml_diff>
--- a/src/main/resources/cardiac_diseases/drools.drl.xlsx
+++ b/src/main/resources/cardiac_diseases/drools.drl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSS\DSS_Cardiac\src\main\resources\cardiac_diseases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CC9797-EAC7-4390-BB02-2340D7FF6E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B2B41D-71E3-4D14-ACFD-485BDE0DB7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="395">
   <si>
     <t>RuleSet</t>
   </si>
@@ -1215,6 +1215,12 @@
   </si>
   <si>
     <t>getSymptoms().contains(Symptom.$param)</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>getSymptoms().size()</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1376,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis6" xfId="1" builtinId="49"/>
@@ -1686,10 +1692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:KM62"/>
+  <dimension ref="A1:KN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="EZ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="FG8" sqref="FG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1839,11 +1845,11 @@
     <col min="154" max="154" width="26" customWidth="1"/>
     <col min="155" max="155" width="38.5546875" customWidth="1"/>
     <col min="156" max="156" width="33.44140625" customWidth="1"/>
-    <col min="157" max="157" width="15.44140625" customWidth="1"/>
-    <col min="158" max="158" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="157" max="158" width="15.44140625" customWidth="1"/>
+    <col min="159" max="159" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -2005,9 +2011,10 @@
       <c r="EY1" s="16"/>
       <c r="EZ1" s="16"/>
       <c r="FA1" s="16"/>
-      <c r="FB1" s="15"/>
+      <c r="FB1" s="16"/>
+      <c r="FC1" s="15"/>
     </row>
-    <row r="2" spans="1:299" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:300" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="17" t="s">
         <v>2</v>
@@ -2170,8 +2177,9 @@
       <c r="EZ2" s="17"/>
       <c r="FA2" s="17"/>
       <c r="FB2" s="17"/>
+      <c r="FC2" s="17"/>
     </row>
-    <row r="3" spans="1:299" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:300" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="17" t="s">
         <v>4</v>
@@ -2334,8 +2342,9 @@
       <c r="EZ3" s="17"/>
       <c r="FA3" s="17"/>
       <c r="FB3" s="17"/>
+      <c r="FC3" s="17"/>
     </row>
-    <row r="4" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:300" x14ac:dyDescent="0.3">
       <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
@@ -2497,11 +2506,12 @@
       <c r="EZ4" s="17"/>
       <c r="FA4" s="17"/>
       <c r="FB4" s="17"/>
+      <c r="FC4" s="17"/>
     </row>
-    <row r="5" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:300" x14ac:dyDescent="0.3">
       <c r="D5" s="20"/>
     </row>
-    <row r="6" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
         <v>8</v>
@@ -2662,8 +2672,9 @@
       <c r="EZ6" s="4"/>
       <c r="FA6" s="4"/>
       <c r="FB6" s="4"/>
+      <c r="FC6" s="4"/>
     </row>
-    <row r="7" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -3136,10 +3147,13 @@
         <v>10</v>
       </c>
       <c r="FB7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="FC7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:299" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:300" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
         <v>12</v>
       </c>
@@ -3298,8 +3312,9 @@
       <c r="EY8" s="21"/>
       <c r="EZ8" s="21"/>
       <c r="FA8" s="21"/>
+      <c r="FB8" s="21"/>
     </row>
-    <row r="9" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:300" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>392</v>
       </c>
@@ -3769,10 +3784,13 @@
         <v>392</v>
       </c>
       <c r="FB9" t="s">
+        <v>394</v>
+      </c>
+      <c r="FC9" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="10" spans="1:299" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:300" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="5" t="s">
         <v>290</v>
@@ -4243,9 +4261,11 @@
         <v>390</v>
       </c>
       <c r="FB10" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="FC10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="FC10"/>
       <c r="FD10"/>
       <c r="FE10"/>
       <c r="FF10"/>
@@ -4386,8 +4406,9 @@
       <c r="KK10"/>
       <c r="KL10"/>
       <c r="KM10"/>
+      <c r="KN10"/>
     </row>
-    <row r="11" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>261</v>
       </c>
@@ -4413,11 +4434,14 @@
       <c r="O11" t="s">
         <v>74</v>
       </c>
-      <c r="FB11" t="s">
+      <c r="FB11">
+        <v>7</v>
+      </c>
+      <c r="FC11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>262</v>
       </c>
@@ -4457,11 +4481,14 @@
       <c r="AD12" s="9"/>
       <c r="AE12" s="9"/>
       <c r="AF12" s="9"/>
-      <c r="FB12" s="6" t="s">
+      <c r="FB12">
+        <v>7</v>
+      </c>
+      <c r="FC12" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>263</v>
       </c>
@@ -4518,11 +4545,14 @@
       <c r="BD13" s="10"/>
       <c r="BE13" s="10"/>
       <c r="BF13" s="10"/>
-      <c r="FB13" s="6" t="s">
+      <c r="FB13">
+        <v>4</v>
+      </c>
+      <c r="FC13" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>88</v>
       </c>
@@ -4590,11 +4620,14 @@
       <c r="BD14" s="10"/>
       <c r="BE14" s="10"/>
       <c r="BF14" s="10"/>
-      <c r="FB14" s="6" t="s">
+      <c r="FB14">
+        <v>11</v>
+      </c>
+      <c r="FC14" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>264</v>
       </c>
@@ -4673,11 +4706,14 @@
       <c r="BD15" s="10"/>
       <c r="BE15" s="10"/>
       <c r="BF15" s="10"/>
-      <c r="FB15" s="6" t="s">
+      <c r="FB15">
+        <v>15</v>
+      </c>
+      <c r="FC15" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:299" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>265</v>
       </c>
@@ -4753,11 +4789,14 @@
       <c r="BD16" s="10"/>
       <c r="BE16" s="10"/>
       <c r="BF16" s="10"/>
-      <c r="FB16" s="6" t="s">
+      <c r="FB16">
+        <v>15</v>
+      </c>
+      <c r="FC16" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>266</v>
       </c>
@@ -4836,11 +4875,14 @@
       <c r="BR17" t="s">
         <v>123</v>
       </c>
-      <c r="FB17" s="6" t="s">
+      <c r="FB17">
+        <v>15</v>
+      </c>
+      <c r="FC17" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>267</v>
       </c>
@@ -4912,11 +4954,14 @@
       <c r="BD18" s="10"/>
       <c r="BE18" s="10"/>
       <c r="BF18" s="10"/>
-      <c r="FB18" s="6" t="s">
+      <c r="FB18">
+        <v>13</v>
+      </c>
+      <c r="FC18" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>268</v>
       </c>
@@ -4994,11 +5039,14 @@
       <c r="CB19" s="10"/>
       <c r="CC19" s="10"/>
       <c r="CD19" s="10"/>
-      <c r="FB19" s="6" t="s">
+      <c r="FB19">
+        <v>6</v>
+      </c>
+      <c r="FC19" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>269</v>
       </c>
@@ -5081,11 +5129,14 @@
       <c r="CB20" s="10"/>
       <c r="CC20" s="10"/>
       <c r="CD20" s="10"/>
-      <c r="FB20" s="6" t="s">
+      <c r="FB20">
+        <v>9</v>
+      </c>
+      <c r="FC20" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>270</v>
       </c>
@@ -5166,11 +5217,14 @@
       <c r="CB21" s="10"/>
       <c r="CC21" s="10"/>
       <c r="CD21" s="10"/>
-      <c r="FB21" s="6" t="s">
+      <c r="FB21">
+        <v>8</v>
+      </c>
+      <c r="FC21" s="6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>271</v>
       </c>
@@ -5252,11 +5306,14 @@
       <c r="CB22" s="10"/>
       <c r="CC22" s="10"/>
       <c r="CD22" s="10"/>
-      <c r="FB22" s="6" t="s">
+      <c r="FB22">
+        <v>8</v>
+      </c>
+      <c r="FC22" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>272</v>
       </c>
@@ -5347,11 +5404,14 @@
       <c r="CB23" s="10"/>
       <c r="CC23" s="10"/>
       <c r="CD23" s="10"/>
-      <c r="FB23" s="6" t="s">
+      <c r="FB23">
+        <v>12</v>
+      </c>
+      <c r="FC23" s="6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>273</v>
       </c>
@@ -5440,11 +5500,14 @@
       <c r="DM24" t="s">
         <v>158</v>
       </c>
-      <c r="FB24" s="6" t="s">
+      <c r="FB24">
+        <v>10</v>
+      </c>
+      <c r="FC24" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>274</v>
       </c>
@@ -5524,11 +5587,14 @@
       <c r="CG25" t="s">
         <v>164</v>
       </c>
-      <c r="FB25" s="6" t="s">
+      <c r="FB25">
+        <v>6</v>
+      </c>
+      <c r="FC25" s="6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>166</v>
       </c>
@@ -5648,11 +5714,14 @@
       <c r="CP26" t="s">
         <v>175</v>
       </c>
-      <c r="FB26" s="6" t="s">
+      <c r="FB26">
+        <v>20</v>
+      </c>
+      <c r="FC26" s="6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>275</v>
       </c>
@@ -5745,11 +5814,14 @@
       <c r="CU27" t="s">
         <v>181</v>
       </c>
-      <c r="FB27" s="6" t="s">
+      <c r="FB27">
+        <v>10</v>
+      </c>
+      <c r="FC27" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>276</v>
       </c>
@@ -5850,11 +5922,14 @@
       <c r="CY28" t="s">
         <v>187</v>
       </c>
-      <c r="FB28" s="6" t="s">
+      <c r="FB28">
+        <v>13</v>
+      </c>
+      <c r="FC28" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>35</v>
       </c>
@@ -5936,11 +6011,14 @@
       <c r="DA29" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="FB29" s="6" t="s">
+      <c r="FB29">
+        <v>7</v>
+      </c>
+      <c r="FC29" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>277</v>
       </c>
@@ -6047,11 +6125,14 @@
       <c r="DI30" t="s">
         <v>198</v>
       </c>
-      <c r="FB30" s="6" t="s">
+      <c r="FB30">
+        <v>16</v>
+      </c>
+      <c r="FC30" s="6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>278</v>
       </c>
@@ -6155,11 +6236,14 @@
       <c r="DN31" t="s">
         <v>203</v>
       </c>
-      <c r="FB31" s="6" t="s">
+      <c r="FB31">
+        <v>15</v>
+      </c>
+      <c r="FC31" s="6" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>205</v>
       </c>
@@ -6266,11 +6350,14 @@
       <c r="DR32" t="s">
         <v>209</v>
       </c>
-      <c r="FB32" s="6" t="s">
+      <c r="FB32">
+        <v>15</v>
+      </c>
+      <c r="FC32" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>211</v>
       </c>
@@ -6393,11 +6480,14 @@
       <c r="DW33" t="s">
         <v>217</v>
       </c>
-      <c r="FB33" s="6" t="s">
+      <c r="FB33">
+        <v>21</v>
+      </c>
+      <c r="FC33" s="6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>279</v>
       </c>
@@ -6482,11 +6572,14 @@
       <c r="EB34" t="s">
         <v>223</v>
       </c>
-      <c r="FB34" s="6" t="s">
+      <c r="FB34">
+        <v>7</v>
+      </c>
+      <c r="FC34" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>280</v>
       </c>
@@ -6588,11 +6681,14 @@
       <c r="EG35" t="s">
         <v>229</v>
       </c>
-      <c r="FB35" s="6" t="s">
+      <c r="FB35">
+        <v>13</v>
+      </c>
+      <c r="FC35" s="6" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>281</v>
       </c>
@@ -6647,11 +6743,14 @@
       <c r="DT36" t="s">
         <v>214</v>
       </c>
-      <c r="FB36" s="6" t="s">
+      <c r="FB36">
+        <v>6</v>
+      </c>
+      <c r="FC36" s="6" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>282</v>
       </c>
@@ -6705,11 +6804,14 @@
       <c r="DH37" t="s">
         <v>197</v>
       </c>
-      <c r="FB37" s="6" t="s">
+      <c r="FB37">
+        <v>6</v>
+      </c>
+      <c r="FC37" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>283</v>
       </c>
@@ -6757,11 +6859,14 @@
       <c r="EH38" t="s">
         <v>233</v>
       </c>
-      <c r="FB38" s="6" t="s">
+      <c r="FB38">
+        <v>3</v>
+      </c>
+      <c r="FC38" s="6" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>284</v>
       </c>
@@ -6828,11 +6933,14 @@
       <c r="EK39" t="s">
         <v>238</v>
       </c>
-      <c r="FB39" s="6" t="s">
+      <c r="FB39">
+        <v>10</v>
+      </c>
+      <c r="FC39" s="6" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="40" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>285</v>
       </c>
@@ -6899,11 +7007,14 @@
       <c r="EO40" t="s">
         <v>243</v>
       </c>
-      <c r="FB40" s="6" t="s">
+      <c r="FB40">
+        <v>10</v>
+      </c>
+      <c r="FC40" s="6" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="41" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>286</v>
       </c>
@@ -6977,11 +7088,14 @@
       <c r="ES41" t="s">
         <v>65</v>
       </c>
-      <c r="FB41" s="6" t="s">
+      <c r="FB41">
+        <v>13</v>
+      </c>
+      <c r="FC41" s="6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="42" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>287</v>
       </c>
@@ -7053,11 +7167,14 @@
       <c r="EU42" t="s">
         <v>250</v>
       </c>
-      <c r="FB42" s="6" t="s">
+      <c r="FB42">
+        <v>12</v>
+      </c>
+      <c r="FC42" s="6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>288</v>
       </c>
@@ -7116,11 +7233,14 @@
       <c r="EV43" t="s">
         <v>252</v>
       </c>
-      <c r="FB43" s="6" t="s">
+      <c r="FB43">
+        <v>7</v>
+      </c>
+      <c r="FC43" s="6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="44" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>289</v>
       </c>
@@ -7176,11 +7296,14 @@
       <c r="FA44" t="s">
         <v>258</v>
       </c>
-      <c r="FB44" s="6" t="s">
+      <c r="FB44">
+        <v>5</v>
+      </c>
+      <c r="FC44" s="6" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="45" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A45" s="17"/>
       <c r="V45" s="9"/>
       <c r="W45" s="9"/>
@@ -7220,7 +7343,7 @@
       <c r="BE45" s="10"/>
       <c r="BF45" s="10"/>
     </row>
-    <row r="46" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:159" x14ac:dyDescent="0.3">
       <c r="V46" s="9"/>
       <c r="W46" s="9"/>
       <c r="X46" s="10"/>
@@ -7259,7 +7382,7 @@
       <c r="BE46" s="10"/>
       <c r="BF46" s="10"/>
     </row>
-    <row r="47" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:159" x14ac:dyDescent="0.3">
       <c r="V47" s="9"/>
       <c r="W47" s="9"/>
       <c r="X47" s="9"/>
@@ -7272,7 +7395,7 @@
       <c r="AE47" s="9"/>
       <c r="AF47" s="9"/>
     </row>
-    <row r="48" spans="1:158" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:159" x14ac:dyDescent="0.3">
       <c r="V48" s="9"/>
       <c r="W48" s="9"/>
       <c r="X48" s="9"/>
@@ -7331,7 +7454,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B8:FA8"/>
+    <mergeCell ref="B8:FB8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change in showPatientInfo and made tests
</commit_message>
<xml_diff>
--- a/src/main/resources/cardiac_diseases/drools.drl.xlsx
+++ b/src/main/resources/cardiac_diseases/drools.drl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSS\DSS_Cardiac\src\main\resources\cardiac_diseases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B2B41D-71E3-4D14-ACFD-485BDE0DB7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD89F12E-9045-4AA0-89E6-6D5AB37D720D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -740,9 +740,6 @@
     <t>CHEYNE_STOKES_BREATHING</t>
   </si>
   <si>
-    <t>REVERSIBLE_CRASH</t>
-  </si>
-  <si>
     <t>DYASTOLIC_SNAP</t>
   </si>
   <si>
@@ -1221,6 +1218,9 @@
   </si>
   <si>
     <t>getSymptoms().size()</t>
+  </si>
+  <si>
+    <t>IRREVERSIBLE_CRASH</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1376,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis6" xfId="1" builtinId="49"/>
@@ -1694,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:KN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EZ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="FG8" sqref="FG8"/>
+    <sheetView tabSelected="1" topLeftCell="EY15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="FC38" sqref="FC38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3316,493 +3316,493 @@
     </row>
     <row r="9" spans="1:300" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="P9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="S9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="T9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="U9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="V9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="X9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Z9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AA9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AB9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AC9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AD9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AE9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AF9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AG9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AH9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AI9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AJ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AK9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AL9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AM9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AN9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AO9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AP9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AQ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AR9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AS9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AT9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AU9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AV9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AW9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AX9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AY9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AZ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BA9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BB9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BC9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BD9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BE9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BF9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BG9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BH9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BI9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BJ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BK9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BL9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BM9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BN9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BO9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BP9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BQ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BR9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BS9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BT9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BU9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BV9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BW9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BX9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BY9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="BZ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CA9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CB9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CC9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CD9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CE9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CF9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CG9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CH9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CI9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CJ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CK9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CL9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CM9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CN9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CO9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CP9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CQ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CR9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CS9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CT9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CU9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CV9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CW9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CX9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CY9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="CZ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DA9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DB9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DC9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DD9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DE9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DF9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DG9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DH9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DI9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DJ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DK9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DL9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DM9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DN9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DO9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DP9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DQ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DR9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DS9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DT9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DU9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DV9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DW9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DX9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DY9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="DZ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EA9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EB9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EC9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="ED9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EE9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EF9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EG9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EH9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EI9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EJ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EK9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EL9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EM9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EN9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EO9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EP9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EQ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="ER9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="ES9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="ET9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EU9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EV9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EW9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EX9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EY9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EZ9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="FA9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="FB9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="FC9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:300" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>293</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>13</v>
@@ -3811,28 +3811,28 @@
         <v>14</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="L10" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="N10" s="4" t="s">
-        <v>300</v>
-      </c>
       <c r="O10" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>15</v>
@@ -3856,7 +3856,7 @@
         <v>21</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>22</v>
@@ -3871,52 +3871,52 @@
         <v>25</v>
       </c>
       <c r="AB10" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="AC10" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="AC10" s="4" t="s">
+      <c r="AD10" s="4" t="s">
         <v>303</v>
-      </c>
-      <c r="AD10" s="4" t="s">
-        <v>304</v>
       </c>
       <c r="AE10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="AF10" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="AG10" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="AG10" s="4" t="s">
-        <v>306</v>
       </c>
       <c r="AH10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="AI10" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="AJ10" s="4" t="s">
         <v>307</v>
-      </c>
-      <c r="AJ10" s="4" t="s">
-        <v>308</v>
       </c>
       <c r="AK10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AL10" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AM10" s="4" t="s">
         <v>29</v>
       </c>
       <c r="AN10" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AO10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="AP10" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="AQ10" s="4" t="s">
-        <v>312</v>
       </c>
       <c r="AR10" s="4" t="s">
         <v>31</v>
@@ -3925,37 +3925,37 @@
         <v>32</v>
       </c>
       <c r="AT10" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="AU10" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="AU10" s="4" t="s">
+      <c r="AV10" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="AV10" s="4" t="s">
+      <c r="AW10" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="AW10" s="4" t="s">
+      <c r="AX10" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="AX10" s="4" t="s">
+      <c r="AY10" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="AY10" s="4" t="s">
+      <c r="AZ10" s="4" t="s">
         <v>318</v>
-      </c>
-      <c r="AZ10" s="4" t="s">
-        <v>319</v>
       </c>
       <c r="BA10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="BB10" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="BC10" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="BC10" s="4" t="s">
+      <c r="BD10" s="4" t="s">
         <v>321</v>
-      </c>
-      <c r="BD10" s="4" t="s">
-        <v>322</v>
       </c>
       <c r="BE10" s="4" t="s">
         <v>34</v>
@@ -3970,49 +3970,49 @@
         <v>37</v>
       </c>
       <c r="BI10" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="BJ10" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="BJ10" s="4" t="s">
+      <c r="BK10" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="BK10" s="4" t="s">
+      <c r="BL10" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="BL10" s="4" t="s">
+      <c r="BM10" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="BM10" s="4" t="s">
+      <c r="BN10" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="BN10" s="4" t="s">
+      <c r="BO10" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="BO10" s="4" t="s">
+      <c r="BP10" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="BP10" s="4" t="s">
+      <c r="BQ10" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="BQ10" s="4" t="s">
+      <c r="BR10" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="BR10" s="4" t="s">
+      <c r="BS10" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="BS10" s="4" t="s">
+      <c r="BT10" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="BT10" s="4" t="s">
+      <c r="BU10" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="BU10" s="4" t="s">
+      <c r="BV10" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="BV10" s="4" t="s">
+      <c r="BW10" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="BW10" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="BX10" s="4" t="s">
         <v>38</v>
@@ -4024,19 +4024,19 @@
         <v>40</v>
       </c>
       <c r="CA10" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="CB10" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="CB10" s="4" t="s">
+      <c r="CC10" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="CC10" s="4" t="s">
+      <c r="CD10" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="CD10" s="4" t="s">
+      <c r="CE10" s="4" t="s">
         <v>341</v>
-      </c>
-      <c r="CE10" s="4" t="s">
-        <v>342</v>
       </c>
       <c r="CF10" s="4" t="s">
         <v>41</v>
@@ -4045,22 +4045,22 @@
         <v>42</v>
       </c>
       <c r="CH10" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="CI10" s="4" t="s">
         <v>43</v>
       </c>
       <c r="CJ10" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="CK10" s="4" t="s">
         <v>44</v>
       </c>
       <c r="CL10" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="CM10" s="4" t="s">
         <v>345</v>
-      </c>
-      <c r="CM10" s="4" t="s">
-        <v>346</v>
       </c>
       <c r="CN10" s="4" t="s">
         <v>45</v>
@@ -4072,22 +4072,22 @@
         <v>47</v>
       </c>
       <c r="CQ10" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="CR10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="CS10" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="CT10" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="CT10" s="4" t="s">
+      <c r="CU10" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="CU10" s="4" t="s">
+      <c r="CV10" s="4" t="s">
         <v>350</v>
-      </c>
-      <c r="CV10" s="4" t="s">
-        <v>351</v>
       </c>
       <c r="CW10" s="4" t="s">
         <v>49</v>
@@ -4096,19 +4096,19 @@
         <v>50</v>
       </c>
       <c r="CY10" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="CZ10" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="CZ10" s="4" t="s">
-        <v>353</v>
       </c>
       <c r="DA10" s="4" t="s">
         <v>51</v>
       </c>
       <c r="DB10" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="DC10" s="4" t="s">
         <v>354</v>
-      </c>
-      <c r="DC10" s="4" t="s">
-        <v>355</v>
       </c>
       <c r="DD10" s="4" t="s">
         <v>52</v>
@@ -4117,10 +4117,10 @@
         <v>53</v>
       </c>
       <c r="DF10" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="DG10" s="4" t="s">
         <v>356</v>
-      </c>
-      <c r="DG10" s="4" t="s">
-        <v>357</v>
       </c>
       <c r="DH10" s="4" t="s">
         <v>54</v>
@@ -4129,34 +4129,34 @@
         <v>55</v>
       </c>
       <c r="DJ10" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="DK10" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="DK10" s="4" t="s">
+      <c r="DL10" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="DL10" s="4" t="s">
+      <c r="DM10" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="DM10" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="DN10" s="4" t="s">
         <v>56</v>
       </c>
       <c r="DO10" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="DP10" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="DP10" s="4" t="s">
+      <c r="DQ10" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="DQ10" s="4" t="s">
+      <c r="DR10" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="DR10" s="4" t="s">
+      <c r="DS10" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="DS10" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="DT10" s="4" t="s">
         <v>57</v>
@@ -4165,73 +4165,73 @@
         <v>58</v>
       </c>
       <c r="DV10" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="DW10" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="DW10" s="4" t="s">
+      <c r="DX10" s="4" t="s">
         <v>368</v>
-      </c>
-      <c r="DX10" s="4" t="s">
-        <v>369</v>
       </c>
       <c r="DY10" s="4" t="s">
         <v>59</v>
       </c>
       <c r="DZ10" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="EA10" s="4" t="s">
         <v>60</v>
       </c>
       <c r="EB10" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="EC10" s="4" t="s">
         <v>61</v>
       </c>
       <c r="ED10" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="EE10" s="4" t="s">
         <v>372</v>
-      </c>
-      <c r="EE10" s="4" t="s">
-        <v>373</v>
       </c>
       <c r="EF10" s="4" t="s">
         <v>62</v>
       </c>
       <c r="EG10" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="EH10" s="4" t="s">
         <v>374</v>
-      </c>
-      <c r="EH10" s="4" t="s">
-        <v>375</v>
       </c>
       <c r="EI10" s="4" t="s">
         <v>63</v>
       </c>
       <c r="EJ10" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="EK10" s="4" t="s">
         <v>376</v>
-      </c>
-      <c r="EK10" s="4" t="s">
-        <v>377</v>
       </c>
       <c r="EL10" s="4" t="s">
         <v>64</v>
       </c>
       <c r="EM10" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="EN10" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="EN10" s="4" t="s">
+      <c r="EO10" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="EO10" s="4" t="s">
+      <c r="EP10" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="EP10" s="4" t="s">
+      <c r="EQ10" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="EQ10" s="4" t="s">
+      <c r="ER10" s="4" t="s">
         <v>382</v>
-      </c>
-      <c r="ER10" s="4" t="s">
-        <v>383</v>
       </c>
       <c r="ES10" s="4" t="s">
         <v>65</v>
@@ -4240,28 +4240,28 @@
         <v>66</v>
       </c>
       <c r="EU10" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="EV10" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="EV10" s="4" t="s">
+      <c r="EW10" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="EW10" s="4" t="s">
+      <c r="EX10" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="EX10" s="4" t="s">
+      <c r="EY10" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="EY10" s="4" t="s">
+      <c r="EZ10" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="EZ10" s="4" t="s">
+      <c r="FA10" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="FA10" s="4" t="s">
-        <v>390</v>
-      </c>
       <c r="FB10" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="FC10" s="4" t="s">
         <v>67</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="11" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>68</v>
@@ -4443,7 +4443,7 @@
     </row>
     <row r="12" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>68</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="13" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B13" s="1"/>
       <c r="D13" t="s">
@@ -4629,7 +4629,7 @@
     </row>
     <row r="15" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4715,7 +4715,7 @@
     </row>
     <row r="16" spans="1:300" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>68</v>
@@ -4798,7 +4798,7 @@
     </row>
     <row r="17" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>68</v>
@@ -4884,7 +4884,7 @@
     </row>
     <row r="18" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>68</v>
@@ -4963,7 +4963,7 @@
     </row>
     <row r="19" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J19" t="s">
         <v>84</v>
@@ -5048,7 +5048,7 @@
     </row>
     <row r="20" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="V20" s="6"/>
       <c r="W20" s="7"/>
@@ -5138,7 +5138,7 @@
     </row>
     <row r="21" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="V21" s="6"/>
       <c r="W21" s="7"/>
@@ -5226,7 +5226,7 @@
     </row>
     <row r="22" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P22" t="s">
         <v>78</v>
@@ -5315,7 +5315,7 @@
     </row>
     <row r="23" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P23" t="s">
         <v>78</v>
@@ -5413,7 +5413,7 @@
     </row>
     <row r="24" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B24" t="s">
         <v>68</v>
@@ -5509,7 +5509,7 @@
     </row>
     <row r="25" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="V25" s="6"/>
       <c r="W25" s="7"/>
@@ -5723,7 +5723,7 @@
     </row>
     <row r="27" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P27" t="s">
         <v>78</v>
@@ -5823,7 +5823,7 @@
     </row>
     <row r="28" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E28" t="s">
         <v>183</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="30" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B30" t="s">
         <v>68</v>
@@ -6134,7 +6134,7 @@
     </row>
     <row r="31" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B31" t="s">
         <v>68</v>
@@ -6489,7 +6489,7 @@
     </row>
     <row r="34" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
@@ -6581,7 +6581,7 @@
     </row>
     <row r="35" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B35" t="s">
         <v>68</v>
@@ -6690,7 +6690,7 @@
     </row>
     <row r="36" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R36" t="s">
         <v>100</v>
@@ -6752,7 +6752,7 @@
     </row>
     <row r="37" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
@@ -6813,7 +6813,7 @@
     </row>
     <row r="38" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="V38" s="9"/>
       <c r="W38" s="9"/>
@@ -6863,12 +6863,12 @@
         <v>3</v>
       </c>
       <c r="FC38" s="6" t="s">
-        <v>234</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O39" t="s">
         <v>74</v>
@@ -6919,30 +6919,30 @@
       <c r="BA39" s="10"/>
       <c r="BB39" s="10"/>
       <c r="BC39" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BD39" s="10"/>
       <c r="BE39" s="10"/>
       <c r="BF39" s="10"/>
       <c r="EI39" t="s">
+        <v>235</v>
+      </c>
+      <c r="EJ39" t="s">
         <v>236</v>
       </c>
-      <c r="EJ39" t="s">
+      <c r="EK39" t="s">
         <v>237</v>
       </c>
-      <c r="EK39" t="s">
+      <c r="FB39">
+        <v>10</v>
+      </c>
+      <c r="FC39" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="FB39">
-        <v>10</v>
-      </c>
-      <c r="FC39" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P40" t="s">
         <v>78</v>
@@ -6996,27 +6996,27 @@
         <v>178</v>
       </c>
       <c r="EL40" t="s">
+        <v>239</v>
+      </c>
+      <c r="EM40" t="s">
         <v>240</v>
       </c>
-      <c r="EM40" t="s">
+      <c r="EN40" t="s">
         <v>241</v>
       </c>
-      <c r="EN40" t="s">
+      <c r="EO40" t="s">
         <v>242</v>
       </c>
-      <c r="EO40" t="s">
+      <c r="FB40">
+        <v>10</v>
+      </c>
+      <c r="FC40" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="FB40">
-        <v>10</v>
-      </c>
-      <c r="FC40" s="6" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P41" t="s">
         <v>78</v>
@@ -7074,16 +7074,16 @@
         <v>209</v>
       </c>
       <c r="EL41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="EP41" t="s">
+        <v>244</v>
+      </c>
+      <c r="EQ41" t="s">
         <v>245</v>
       </c>
-      <c r="EQ41" t="s">
+      <c r="ER41" t="s">
         <v>246</v>
-      </c>
-      <c r="ER41" t="s">
-        <v>247</v>
       </c>
       <c r="ES41" t="s">
         <v>65</v>
@@ -7092,12 +7092,12 @@
         <v>13</v>
       </c>
       <c r="FC41" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P42" t="s">
         <v>78</v>
@@ -7150,7 +7150,7 @@
       <c r="BE42" s="10"/>
       <c r="BF42" s="10"/>
       <c r="BT42" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="DD42" t="s">
         <v>193</v>
@@ -7159,24 +7159,24 @@
         <v>209</v>
       </c>
       <c r="EL42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="ET42" t="s">
         <v>66</v>
       </c>
       <c r="EU42" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="FB42">
         <v>12</v>
       </c>
       <c r="FC42" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B43" t="s">
         <v>68</v>
@@ -7228,21 +7228,21 @@
       <c r="BE43" s="10"/>
       <c r="BF43" s="10"/>
       <c r="ER43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="EV43" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="FB43">
         <v>7</v>
       </c>
       <c r="FC43" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="V44" s="9"/>
       <c r="W44" s="9"/>
@@ -7282,25 +7282,25 @@
       <c r="BE44" s="10"/>
       <c r="BF44" s="10"/>
       <c r="EW44" t="s">
+        <v>253</v>
+      </c>
+      <c r="EX44" t="s">
         <v>254</v>
       </c>
-      <c r="EX44" t="s">
+      <c r="EY44" t="s">
         <v>255</v>
       </c>
-      <c r="EY44" t="s">
+      <c r="EZ44" t="s">
         <v>256</v>
       </c>
-      <c r="EZ44" t="s">
+      <c r="FA44" t="s">
         <v>257</v>
-      </c>
-      <c r="FA44" t="s">
-        <v>258</v>
       </c>
       <c r="FB44">
         <v>5</v>
       </c>
       <c r="FC44" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:159" x14ac:dyDescent="0.3">
@@ -7461,20 +7461,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7c9ee31f-ab73-4c39-aa9f-17155d47e22c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7c9ee31f-ab73-4c39-aa9f-17155d47e22c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7699,19 +7699,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C81BB3D-3712-4086-AD03-5503951DDC8A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0B1BFB-4AD7-47D5-9509-41A4ECBCCE64}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7c9ee31f-ab73-4c39-aa9f-17155d47e22c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0B1BFB-4AD7-47D5-9509-41A4ECBCCE64}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C81BB3D-3712-4086-AD03-5503951DDC8A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7c9ee31f-ab73-4c39-aa9f-17155d47e22c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>